<commit_message>
Add type to single issues Changed config for data fields changed data fields to display
@time: 2h
</commit_message>
<xml_diff>
--- a/goobi-plugin-administration-nli-dailypress/test/resources/BatchDepositSample.xlsx
+++ b/goobi-plugin-administration-nli-dailypress/test/resources/BatchDepositSample.xlsx
@@ -24,19 +24,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
-    <t xml:space="preserve">code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">issue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type</t>
+    <t xml:space="preserve">Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
   </si>
   <si>
     <t xml:space="preserve">12-54</t>
@@ -178,17 +178,17 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.5813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.47441860465116"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.0744186046512"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="17.7209302325581"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.47441860465116"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.72093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="18.2139534883721"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.72093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -317,7 +317,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -343,7 +343,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>